<commit_message>
Incluyendo G y Aast
</commit_message>
<xml_diff>
--- a/codigo/vigas/Euler-Bernoulli/viga_Uribe_Escamilla_ej_5_5.xlsx
+++ b/codigo/vigas/Euler-Bernoulli/viga_Uribe_Escamilla_ej_5_5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,12 +18,15 @@
     <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="b" vbProcedure="false">LaG_EI_q!$J$2</definedName>
-    <definedName function="false" hidden="false" name="E" vbProcedure="false">LaG_EI_q!$J$4</definedName>
-    <definedName function="false" hidden="false" name="h" vbProcedure="false">LaG_EI_q!$J$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="b" vbProcedure="false">[2]LaG_EI_q!$J$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="E" vbProcedure="false">[2]LaG_EI_q!$J$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="h" vbProcedure="false">[2]LaG_EI_q!$J$3</definedName>
+    <definedName function="false" hidden="false" name="alpha" vbProcedure="false">LaG_EI_q!$L$7</definedName>
+    <definedName function="false" hidden="false" name="b" vbProcedure="false">LaG_EI_q!$L$2</definedName>
+    <definedName function="false" hidden="false" name="E" vbProcedure="false">LaG_EI_q!$L$4</definedName>
+    <definedName function="false" hidden="false" name="G" vbProcedure="false">LaG_EI_q!$L$6</definedName>
+    <definedName function="false" hidden="false" name="h" vbProcedure="false">LaG_EI_q!$L$3</definedName>
+    <definedName function="false" hidden="false" name="nu" vbProcedure="false">LaG_EI_q!$L$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="b" vbProcedure="false">[1]LaG_EI_q!$J$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="E" vbProcedure="false">[1]LaG_EI_q!$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="h" vbProcedure="false">[1]LaG_EI_q!$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,11 +47,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <family val="1"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">m</t>
+          <t>m</t>
         </r>
       </text>
     </comment>
@@ -66,12 +71,13 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <family val="1"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">kPa</t>
+          <t>kPa</t>
         </r>
       </text>
     </comment>
@@ -79,12 +85,13 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <family val="1"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">m^4</t>
+          <t>m^4</t>
         </r>
       </text>
     </comment>
@@ -92,12 +99,13 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <family val="1"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">kN/m</t>
+          <t>kPa</t>
         </r>
       </text>
     </comment>
@@ -105,12 +113,41 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <family val="1"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">kN/m</t>
+          <t>m^2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t>kN/m</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t>kN/m</t>
         </r>
       </text>
     </comment>
@@ -128,11 +165,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <family val="1"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">m o radianes</t>
+          <t>m o radianes</t>
         </r>
       </text>
     </comment>
@@ -150,12 +189,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
+            <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">kN</t>
+          <t>kN</t>
         </r>
       </text>
     </comment>
@@ -173,12 +213,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
+            <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">kN o kN-m</t>
+          <t>kN o kN-m</t>
         </r>
       </text>
     </comment>
@@ -187,81 +228,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
-    <t xml:space="preserve">nodo</t>
+    <t>nodo</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
+    <t>x</t>
   </si>
   <si>
-    <t xml:space="preserve">Viga analizada en el Ejemplo 5-5 de Uribe Escamilla</t>
+    <t>Viga analizada en el Ejemplo 5-5 de Uribe Escamilla</t>
   </si>
   <si>
-    <t xml:space="preserve">Unidades en kN y m</t>
+    <t>Unidades en kN y m</t>
   </si>
   <si>
-    <t xml:space="preserve">EF</t>
+    <t>EF</t>
   </si>
   <si>
-    <t xml:space="preserve">NL1</t>
+    <t>NL1</t>
   </si>
   <si>
-    <t xml:space="preserve">NL2</t>
+    <t>NL2</t>
   </si>
   <si>
-    <t xml:space="preserve">E</t>
+    <t>E</t>
   </si>
   <si>
-    <t xml:space="preserve">I</t>
+    <t>I</t>
   </si>
   <si>
-    <t xml:space="preserve">q1e</t>
+    <t>G</t>
   </si>
   <si>
-    <t xml:space="preserve">q2e</t>
+    <t>Aast</t>
   </si>
   <si>
-    <t xml:space="preserve">b =</t>
+    <t>q1e</t>
   </si>
   <si>
-    <t xml:space="preserve">m</t>
+    <t>q2e</t>
   </si>
   <si>
-    <t xml:space="preserve">h = </t>
+    <t>b =</t>
   </si>
   <si>
-    <t xml:space="preserve">E = </t>
+    <t>m</t>
   </si>
   <si>
-    <t xml:space="preserve">kPa</t>
+    <t>h = </t>
   </si>
   <si>
-    <t xml:space="preserve">direccion</t>
+    <t>E = </t>
   </si>
   <si>
-    <t xml:space="preserve">desplazamiento</t>
+    <t>kPa</t>
   </si>
   <si>
-    <t xml:space="preserve">Y = 1</t>
+    <t>nu =</t>
   </si>
   <si>
-    <t xml:space="preserve">TH = 2</t>
+    <t>G =</t>
   </si>
   <si>
-    <t xml:space="preserve">rad</t>
+    <t>alpha = </t>
   </si>
   <si>
-    <t xml:space="preserve">fuerza_puntual</t>
+    <t>direccion</t>
   </si>
   <si>
-    <t xml:space="preserve">kN</t>
+    <t>desplazamiento</t>
   </si>
   <si>
-    <t xml:space="preserve">tipo</t>
+    <t>Y = 1</t>
   </si>
   <si>
-    <t xml:space="preserve">k</t>
+    <t>TH = 2</t>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t>fuerza_puntual</t>
+  </si>
+  <si>
+    <t>kN</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -269,11 +325,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.0_ "/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -305,17 +361,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -325,12 +370,6 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -402,15 +441,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -431,15 +470,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>409680</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1800</xdr:rowOff>
+      <xdr:colOff>463680</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>218880</xdr:colOff>
+      <xdr:colOff>272160</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -452,8 +491,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647720" y="1437840"/>
-          <a:ext cx="6619680" cy="7610400"/>
+          <a:off x="2025720" y="1419840"/>
+          <a:ext cx="8399880" cy="7609680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -468,7 +507,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -481,13 +520,13 @@
   </sheetPr>
   <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q19" activeCellId="0" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,23 +2089,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K191"/>
+  <dimension ref="A1:M191"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7975708502024"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2088,8 +2128,14 @@
       <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -2107,17 +2153,25 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="0" t="n">
+      <c r="F2" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -2135,17 +2189,25 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="0" t="n">
+      <c r="F3" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -2163,17 +2225,25 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>200000000</v>
+      <c r="F4" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>200000000</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -2191,8 +2261,22 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -2210,8 +2294,23 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">E/(2*(1+nu))</f>
+        <v>76923076.9230769</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -2229,8 +2328,23 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <f aca="false">5/6</f>
+        <v>0.833333333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -2248,8 +2362,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
@@ -2267,8 +2389,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -2286,8 +2416,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -2305,8 +2443,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
@@ -2324,8 +2470,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
@@ -2343,8 +2497,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -2362,8 +2524,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
@@ -2381,8 +2551,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
@@ -2400,8 +2578,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
@@ -2419,8 +2605,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
@@ -2438,8 +2632,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
@@ -2457,8 +2659,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
@@ -2476,8 +2686,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
@@ -2495,8 +2713,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
@@ -2514,8 +2740,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
@@ -2533,8 +2767,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
@@ -2552,8 +2794,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
@@ -2571,8 +2821,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
@@ -2590,8 +2848,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
@@ -2609,8 +2875,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
@@ -2628,8 +2902,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F28" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
@@ -2647,8 +2929,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F29" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
@@ -2666,8 +2956,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
@@ -2685,8 +2983,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
@@ -2704,8 +3010,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
@@ -2723,8 +3037,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F33" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
@@ -2742,8 +3064,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F34" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
@@ -2761,8 +3091,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F35" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
@@ -2780,8 +3118,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F36" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
@@ -2799,8 +3145,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
@@ -2818,8 +3172,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F38" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
@@ -2837,8 +3199,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
@@ -2856,8 +3226,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F40" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
@@ -2875,8 +3253,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F41" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
@@ -2894,8 +3280,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F42" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
@@ -2913,8 +3307,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F43" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
@@ -2932,8 +3334,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F44" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
@@ -2951,8 +3361,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F45" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
@@ -2970,8 +3388,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F46" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
@@ -2989,8 +3415,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F47" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
@@ -3008,8 +3442,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F48" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
@@ -3027,8 +3469,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F49" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
@@ -3046,8 +3496,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F50" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
@@ -3065,8 +3523,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F51" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>51</v>
       </c>
@@ -3084,8 +3550,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F52" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>52</v>
       </c>
@@ -3103,8 +3577,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F53" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
@@ -3122,8 +3604,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F54" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
@@ -3141,8 +3631,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F55" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
@@ -3160,8 +3658,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F56" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>56</v>
       </c>
@@ -3179,8 +3685,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F57" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
@@ -3198,8 +3712,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F58" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
@@ -3217,8 +3739,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F59" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
@@ -3236,8 +3766,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F60" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
@@ -3255,8 +3793,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F61" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
@@ -3274,8 +3820,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F62" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
@@ -3293,8 +3847,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F63" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
@@ -3312,8 +3874,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F64" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
@@ -3331,8 +3901,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F65" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
@@ -3350,8 +3928,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F66" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
@@ -3369,8 +3955,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F67" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
@@ -3388,8 +3982,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F68" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
@@ -3407,8 +4009,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F69" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
@@ -3426,8 +4036,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F70" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
@@ -3445,8 +4063,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F71" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
@@ -3464,8 +4090,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F72" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
@@ -3483,8 +4117,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F73" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>73</v>
       </c>
@@ -3502,8 +4144,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F74" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>74</v>
       </c>
@@ -3521,8 +4171,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F75" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>75</v>
       </c>
@@ -3540,8 +4198,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F76" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>76</v>
       </c>
@@ -3559,8 +4225,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F77" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>77</v>
       </c>
@@ -3578,8 +4252,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F78" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
@@ -3597,8 +4279,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F79" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>79</v>
       </c>
@@ -3616,8 +4306,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F80" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>80</v>
       </c>
@@ -3635,8 +4333,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F81" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>81</v>
       </c>
@@ -3654,8 +4360,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F82" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>82</v>
       </c>
@@ -3673,8 +4387,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F83" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>83</v>
       </c>
@@ -3692,8 +4414,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F84" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>84</v>
       </c>
@@ -3711,8 +4441,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F85" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>85</v>
       </c>
@@ -3730,8 +4468,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F86" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G86" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>86</v>
       </c>
@@ -3749,8 +4495,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F87" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G87" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>87</v>
       </c>
@@ -3768,8 +4522,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F88" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G88" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>88</v>
       </c>
@@ -3787,8 +4549,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F89" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G89" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>89</v>
       </c>
@@ -3806,8 +4576,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F90" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G90" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>90</v>
       </c>
@@ -3825,8 +4603,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F91" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G91" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>91</v>
       </c>
@@ -3844,8 +4630,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F92" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G92" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>92</v>
       </c>
@@ -3863,8 +4657,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F93" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G93" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>93</v>
       </c>
@@ -3882,8 +4684,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F94" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G94" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <v>94</v>
       </c>
@@ -3901,8 +4711,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F95" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G95" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>95</v>
       </c>
@@ -3920,8 +4738,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F96" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G96" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <v>96</v>
       </c>
@@ -3939,8 +4765,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F97" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G97" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <v>97</v>
       </c>
@@ -3958,8 +4792,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F98" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G98" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <v>98</v>
       </c>
@@ -3977,8 +4819,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F99" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G99" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>99</v>
       </c>
@@ -3996,8 +4846,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F100" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G100" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
         <v>100</v>
       </c>
@@ -4015,8 +4873,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F101" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G101" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
         <v>101</v>
       </c>
@@ -4035,13 +4901,21 @@
         <v>0.084375</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G102" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H102" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I102" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
         <v>102</v>
       </c>
@@ -4060,13 +4934,21 @@
         <v>0.084375</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G103" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H103" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I103" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
         <v>103</v>
       </c>
@@ -4085,13 +4967,21 @@
         <v>0.084375</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G104" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H104" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I104" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
         <v>104</v>
       </c>
@@ -4110,13 +5000,21 @@
         <v>0.084375</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G105" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H105" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I105" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
         <v>105</v>
       </c>
@@ -4135,13 +5033,21 @@
         <v>0.084375</v>
       </c>
       <c r="F106" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G106" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H106" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I106" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
         <v>106</v>
       </c>
@@ -4160,13 +5066,21 @@
         <v>0.084375</v>
       </c>
       <c r="F107" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G107" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H107" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I107" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
         <v>107</v>
       </c>
@@ -4185,13 +5099,21 @@
         <v>0.084375</v>
       </c>
       <c r="F108" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G108" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H108" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I108" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
         <v>108</v>
       </c>
@@ -4210,13 +5132,21 @@
         <v>0.084375</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G109" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H109" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I109" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
         <v>109</v>
       </c>
@@ -4235,13 +5165,21 @@
         <v>0.084375</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G110" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H110" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I110" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
         <v>110</v>
       </c>
@@ -4260,13 +5198,21 @@
         <v>0.084375</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G111" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H111" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I111" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
         <v>111</v>
       </c>
@@ -4285,13 +5231,21 @@
         <v>0.084375</v>
       </c>
       <c r="F112" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G112" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H112" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I112" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
         <v>112</v>
       </c>
@@ -4310,13 +5264,21 @@
         <v>0.084375</v>
       </c>
       <c r="F113" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G113" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H113" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I113" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
         <v>113</v>
       </c>
@@ -4335,13 +5297,21 @@
         <v>0.084375</v>
       </c>
       <c r="F114" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G114" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H114" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I114" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
         <v>114</v>
       </c>
@@ -4360,13 +5330,21 @@
         <v>0.084375</v>
       </c>
       <c r="F115" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G115" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H115" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I115" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
         <v>115</v>
       </c>
@@ -4385,13 +5363,21 @@
         <v>0.084375</v>
       </c>
       <c r="F116" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G116" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H116" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I116" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
         <v>116</v>
       </c>
@@ -4410,13 +5396,21 @@
         <v>0.084375</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G117" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H117" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I117" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
         <v>117</v>
       </c>
@@ -4435,13 +5429,21 @@
         <v>0.084375</v>
       </c>
       <c r="F118" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G118" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H118" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I118" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
         <v>118</v>
       </c>
@@ -4460,13 +5462,21 @@
         <v>0.084375</v>
       </c>
       <c r="F119" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G119" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H119" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I119" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
         <v>119</v>
       </c>
@@ -4485,13 +5495,21 @@
         <v>0.084375</v>
       </c>
       <c r="F120" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G120" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H120" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I120" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
         <v>120</v>
       </c>
@@ -4510,13 +5528,21 @@
         <v>0.084375</v>
       </c>
       <c r="F121" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G121" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H121" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I121" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
         <v>121</v>
       </c>
@@ -4535,13 +5561,21 @@
         <v>0.084375</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G122" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H122" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I122" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
         <v>122</v>
       </c>
@@ -4560,13 +5594,21 @@
         <v>0.084375</v>
       </c>
       <c r="F123" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G123" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H123" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I123" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
         <v>123</v>
       </c>
@@ -4585,13 +5627,21 @@
         <v>0.084375</v>
       </c>
       <c r="F124" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G124" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H124" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I124" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
         <v>124</v>
       </c>
@@ -4610,13 +5660,21 @@
         <v>0.084375</v>
       </c>
       <c r="F125" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G125" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H125" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I125" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="n">
         <v>125</v>
       </c>
@@ -4635,13 +5693,21 @@
         <v>0.084375</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G126" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H126" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I126" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
         <v>126</v>
       </c>
@@ -4660,13 +5726,21 @@
         <v>0.084375</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G127" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H127" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I127" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
         <v>127</v>
       </c>
@@ -4685,13 +5759,21 @@
         <v>0.084375</v>
       </c>
       <c r="F128" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G128" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H128" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I128" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
         <v>128</v>
       </c>
@@ -4710,13 +5792,21 @@
         <v>0.084375</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G129" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H129" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I129" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="n">
         <v>129</v>
       </c>
@@ -4735,13 +5825,21 @@
         <v>0.084375</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G130" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H130" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I130" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="n">
         <v>130</v>
       </c>
@@ -4760,13 +5858,21 @@
         <v>0.084375</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G131" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H131" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I131" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="n">
         <v>131</v>
       </c>
@@ -4785,13 +5891,21 @@
         <v>0.084375</v>
       </c>
       <c r="F132" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G132" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H132" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I132" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="n">
         <v>132</v>
       </c>
@@ -4810,13 +5924,21 @@
         <v>0.084375</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G133" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H133" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I133" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
         <v>133</v>
       </c>
@@ -4835,13 +5957,21 @@
         <v>0.084375</v>
       </c>
       <c r="F134" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G134" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H134" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I134" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="n">
         <v>134</v>
       </c>
@@ -4860,13 +5990,21 @@
         <v>0.084375</v>
       </c>
       <c r="F135" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G135" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H135" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I135" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="n">
         <v>135</v>
       </c>
@@ -4885,13 +6023,21 @@
         <v>0.084375</v>
       </c>
       <c r="F136" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G136" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H136" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I136" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="n">
         <v>136</v>
       </c>
@@ -4910,13 +6056,21 @@
         <v>0.084375</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G137" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H137" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I137" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="n">
         <v>137</v>
       </c>
@@ -4935,13 +6089,21 @@
         <v>0.084375</v>
       </c>
       <c r="F138" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G138" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H138" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I138" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="n">
         <v>138</v>
       </c>
@@ -4960,13 +6122,21 @@
         <v>0.084375</v>
       </c>
       <c r="F139" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G139" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H139" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I139" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="n">
         <v>139</v>
       </c>
@@ -4985,13 +6155,21 @@
         <v>0.084375</v>
       </c>
       <c r="F140" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G140" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H140" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I140" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="n">
         <v>140</v>
       </c>
@@ -5010,13 +6188,21 @@
         <v>0.084375</v>
       </c>
       <c r="F141" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G141" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H141" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I141" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="n">
         <v>141</v>
       </c>
@@ -5035,13 +6221,21 @@
         <v>0.084375</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G142" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H142" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I142" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="n">
         <v>142</v>
       </c>
@@ -5060,13 +6254,21 @@
         <v>0.084375</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G143" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H143" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I143" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="n">
         <v>143</v>
       </c>
@@ -5085,13 +6287,21 @@
         <v>0.084375</v>
       </c>
       <c r="F144" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G144" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H144" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I144" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
         <v>144</v>
       </c>
@@ -5110,13 +6320,21 @@
         <v>0.084375</v>
       </c>
       <c r="F145" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G145" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H145" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I145" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="n">
         <v>145</v>
       </c>
@@ -5135,13 +6353,21 @@
         <v>0.084375</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G146" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H146" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I146" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
         <v>146</v>
       </c>
@@ -5160,13 +6386,21 @@
         <v>0.084375</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G147" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H147" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I147" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
         <v>147</v>
       </c>
@@ -5185,13 +6419,21 @@
         <v>0.084375</v>
       </c>
       <c r="F148" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G148" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H148" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I148" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
         <v>148</v>
       </c>
@@ -5210,13 +6452,21 @@
         <v>0.084375</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G149" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H149" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I149" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
         <v>149</v>
       </c>
@@ -5235,13 +6485,21 @@
         <v>0.084375</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G150" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H150" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I150" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
         <v>150</v>
       </c>
@@ -5260,13 +6518,21 @@
         <v>0.084375</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G151" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H151" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I151" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
         <v>151</v>
       </c>
@@ -5285,13 +6551,21 @@
         <v>0.084375</v>
       </c>
       <c r="F152" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G152" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H152" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I152" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
         <v>152</v>
       </c>
@@ -5310,13 +6584,21 @@
         <v>0.084375</v>
       </c>
       <c r="F153" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G153" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H153" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I153" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
         <v>153</v>
       </c>
@@ -5335,13 +6617,21 @@
         <v>0.084375</v>
       </c>
       <c r="F154" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G154" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H154" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I154" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="n">
         <v>154</v>
       </c>
@@ -5360,13 +6650,21 @@
         <v>0.084375</v>
       </c>
       <c r="F155" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G155" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H155" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I155" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
         <v>155</v>
       </c>
@@ -5385,13 +6683,21 @@
         <v>0.084375</v>
       </c>
       <c r="F156" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G156" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H156" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I156" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="n">
         <v>156</v>
       </c>
@@ -5410,13 +6716,21 @@
         <v>0.084375</v>
       </c>
       <c r="F157" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G157" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H157" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I157" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
         <v>157</v>
       </c>
@@ -5435,13 +6749,21 @@
         <v>0.084375</v>
       </c>
       <c r="F158" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G158" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H158" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I158" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
         <v>158</v>
       </c>
@@ -5460,13 +6782,21 @@
         <v>0.084375</v>
       </c>
       <c r="F159" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G159" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H159" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I159" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
         <v>159</v>
       </c>
@@ -5485,13 +6815,21 @@
         <v>0.084375</v>
       </c>
       <c r="F160" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G160" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H160" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I160" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
         <v>160</v>
       </c>
@@ -5510,13 +6848,21 @@
         <v>0.084375</v>
       </c>
       <c r="F161" s="0" t="n">
-        <v>-12</v>
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
       </c>
       <c r="G161" s="0" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+      <c r="H161" s="0" t="n">
+        <v>-12</v>
+      </c>
+      <c r="I161" s="0" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
         <v>161</v>
       </c>
@@ -5534,8 +6880,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F162" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G162" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
         <v>162</v>
       </c>
@@ -5553,8 +6907,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F163" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G163" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="n">
         <v>163</v>
       </c>
@@ -5572,8 +6934,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F164" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G164" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="n">
         <v>164</v>
       </c>
@@ -5591,8 +6961,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F165" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G165" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="n">
         <v>165</v>
       </c>
@@ -5610,8 +6988,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F166" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G166" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
         <v>166</v>
       </c>
@@ -5629,8 +7015,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F167" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G167" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
         <v>167</v>
       </c>
@@ -5648,8 +7042,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F168" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G168" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
         <v>168</v>
       </c>
@@ -5667,8 +7069,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F169" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G169" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
         <v>169</v>
       </c>
@@ -5686,8 +7096,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F170" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G170" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
         <v>170</v>
       </c>
@@ -5705,8 +7123,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F171" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G171" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
         <v>171</v>
       </c>
@@ -5724,8 +7150,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F172" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G172" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
         <v>172</v>
       </c>
@@ -5743,8 +7177,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F173" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G173" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
         <v>173</v>
       </c>
@@ -5762,8 +7204,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F174" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G174" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
         <v>174</v>
       </c>
@@ -5781,8 +7231,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F175" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G175" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="n">
         <v>175</v>
       </c>
@@ -5800,8 +7258,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F176" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G176" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="n">
         <v>176</v>
       </c>
@@ -5819,8 +7285,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F177" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G177" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="n">
         <v>177</v>
       </c>
@@ -5838,8 +7312,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F178" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G178" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="n">
         <v>178</v>
       </c>
@@ -5857,8 +7339,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F179" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G179" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="n">
         <v>179</v>
       </c>
@@ -5876,8 +7366,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F180" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G180" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="n">
         <v>180</v>
       </c>
@@ -5895,8 +7393,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F181" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G181" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="n">
         <v>181</v>
       </c>
@@ -5914,8 +7420,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F182" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G182" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="n">
         <v>182</v>
       </c>
@@ -5933,8 +7447,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F183" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G183" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="n">
         <v>183</v>
       </c>
@@ -5952,8 +7474,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F184" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G184" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="n">
         <v>184</v>
       </c>
@@ -5971,8 +7501,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F185" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G185" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="n">
         <v>185</v>
       </c>
@@ -5990,8 +7528,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F186" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G186" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
         <v>186</v>
       </c>
@@ -6009,8 +7555,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="188" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F187" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G187" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
         <v>187</v>
       </c>
@@ -6028,8 +7582,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="189" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F188" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G188" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
         <v>188</v>
       </c>
@@ -6047,8 +7609,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="190" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F189" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G189" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="n">
         <v>189</v>
       </c>
@@ -6066,8 +7636,16 @@
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
       </c>
-    </row>
-    <row r="191" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F190" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G190" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="n">
         <v>190</v>
       </c>
@@ -6084,6 +7662,14 @@
       <c r="E191" s="0" t="n">
         <f aca="false">b*h^3/12</f>
         <v>0.084375</v>
+      </c>
+      <c r="F191" s="0" t="n">
+        <f aca="false">G</f>
+        <v>76923076.9230769</v>
+      </c>
+      <c r="G191" s="0" t="n">
+        <f aca="false">alpha*b*h</f>
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>
@@ -6111,7 +7697,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6119,16 +7705,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6142,7 +7728,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -6158,7 +7744,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -6174,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6188,7 +7774,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -6216,9 +7802,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="5" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6226,17 +7812,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D1" s="0"/>
       <c r="F1" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6250,7 +7836,7 @@
         <v>-30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6264,7 +7850,7 @@
         <v>-15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -6292,7 +7878,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6300,17 +7886,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G1" s="5"/>
     </row>

</xml_diff>